<commit_message>
added generation of unique pairs
</commit_message>
<xml_diff>
--- a/analysis/pairing matrix scenarios.xlsx
+++ b/analysis/pairing matrix scenarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>anette</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>rich &amp; khali</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anette &amp; rich</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rick &amp; khali</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>anette &amp; khali</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rick &amp; rich</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>round 5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -426,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -447,29 +471,47 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>3</v>
       </c>

</xml_diff>